<commit_message>
fixingt tables in rdas
</commit_message>
<xml_diff>
--- a/County-SO-Data/Garfield/Garfield.xlsx
+++ b/County-SO-Data/Garfield/Garfield.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidris\Documents\GitHub\wa-pursuit-pdr-data\County-SO-Data\Garfield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB8625F-C14F-4AD8-A386-0E513D15B27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91808289-A095-440D-83DB-79106AE43C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2350" yWindow="1090" windowWidth="14400" windowHeight="7360" xr2:uid="{F532931A-81D9-4211-B6C6-93AE5F82B6BC}"/>
+    <workbookView xWindow="3510" yWindow="1310" windowWidth="14400" windowHeight="7360" xr2:uid="{F532931A-81D9-4211-B6C6-93AE5F82B6BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Year</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Number of incidents</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -416,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B410FAA-A0CA-46B3-B3BA-E7BDBBAC5EE0}">
-  <dimension ref="A2:M8"/>
+  <dimension ref="A2:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -432,7 +435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -472,16 +475,23 @@
       <c r="M3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2019</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4">
+        <f>SUM(B4:M4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -491,29 +501,102 @@
       <c r="K5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <f t="shared" ref="N5:N9" si="0">SUM(B5:M5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2021</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2022</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2023</v>
       </c>
       <c r="E8">
         <v>1</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B4:B8)</f>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:I9" si="1">SUM(C4:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f>SUM(J4:J8)</f>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9" si="2">SUM(K4:K8)</f>
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9" si="3">SUM(L4:L8)</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:N9" si="4">SUM(M4:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>